<commit_message>
fix excel file error;
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/BB_Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/BB_Player.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19560" windowHeight="8460" activeTab="2"/>
+    <workbookView windowWidth="18870" windowHeight="8550" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -36,7 +36,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +85,7 @@
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
   <si>
     <t>Id</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Col</t>
+  </si>
+  <si>
+    <t>View</t>
   </si>
   <si>
     <t>MonsterID</t>
@@ -254,22 +257,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
       <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -294,19 +292,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1033,10 +1031,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -1045,16 +1043,16 @@
     <col min="2" max="3" width="7.125" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="9.375" customWidth="1"/>
-    <col min="8" max="8" width="17.75" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="12.75" customWidth="1"/>
-    <col min="12" max="13" width="22.75" customWidth="1"/>
-    <col min="14" max="14" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="9.375" customWidth="1"/>
+    <col min="9" max="9" width="17.75" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="12.75" customWidth="1"/>
+    <col min="13" max="14" width="22.75" customWidth="1"/>
+    <col min="15" max="15" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1074,19 +1072,19 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>36</v>
       </c>
       <c r="L1" t="s">
         <v>37</v>
@@ -1097,10 +1095,13 @@
       <c r="N1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -1117,41 +1118,45 @@
       <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="G2" t="b">
+        <v>1</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" t="s">
         <v>10</v>
-      </c>
-      <c r="L2" t="s">
-        <v>14</v>
       </c>
       <c r="M2" t="s">
         <v>14</v>
       </c>
       <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="K:N">
-      <formula1>"int,float,string,object"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D:F">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D:F">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1"/>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B:C">
       <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L:O">
+      <formula1>"int,float,string,object"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1164,10 +1169,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -1176,14 +1181,14 @@
     <col min="2" max="3" width="7.125" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="9.375" customWidth="1"/>
-    <col min="8" max="8" width="17.125" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="11" max="11" width="12.75" customWidth="1"/>
-    <col min="12" max="12" width="13.875" customWidth="1"/>
+    <col min="8" max="8" width="9.375" customWidth="1"/>
+    <col min="9" max="9" width="17.125" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="12" max="12" width="12.75" customWidth="1"/>
+    <col min="13" max="13" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1203,33 +1208,36 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>42</v>
       </c>
       <c r="L1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>128</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -1240,31 +1248,35 @@
       <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="G2" t="b">
+        <v>1</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
+      <c r="K2" s="1"/>
       <c r="L2" t="s">
         <v>10</v>
       </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="K1:L1 K42:K1048576"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L2 K2:K41">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D:F">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1:M1 L42:L1048576"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M2 L2:L41">
       <formula1>"int,float,string,object"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D:F">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B:C">
       <formula1>0</formula1>
@@ -1295,13 +1307,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
modified enum of record[guild]
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/BB_Player.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/BB_Player.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Struct\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
+    <workbookView windowWidth="19560" windowHeight="8460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
-    <sheet name="Record_TaskMonsterList" sheetId="2" r:id="rId2"/>
-    <sheet name="Record_BuildingList" sheetId="3" r:id="rId3"/>
-    <sheet name="Record_BuildingProduce" sheetId="5" r:id="rId4"/>
-    <sheet name="Component" sheetId="4" r:id="rId5"/>
+    <sheet name="Record_BuildingList" sheetId="2" r:id="rId2"/>
+    <sheet name="Record_BuildingProduce" sheetId="3" r:id="rId3"/>
+    <sheet name="Component" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -28,83 +22,16 @@
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
-            <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>物品配置ID</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>强化等级</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>镶嵌宝石，逗号分隔</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>附魔等级</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>pengbo.yang</author>
-  </authors>
-  <commentList>
-    <comment ref="L1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>建筑ID</t>
+          <t xml:space="preserve">建筑ID</t>
         </r>
       </text>
     </comment>
@@ -113,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56">
   <si>
     <t>Id</t>
   </si>
@@ -220,33 +147,60 @@
     <t>拥有的钻石</t>
   </si>
   <si>
+    <t>LoadPropertyFinish</t>
+  </si>
+  <si>
     <t>Row</t>
   </si>
   <si>
     <t>Col</t>
   </si>
   <si>
-    <t>MonsterID</t>
-  </si>
-  <si>
-    <t>CurrentKillCount</t>
-  </si>
-  <si>
-    <t>RequireKillCount</t>
-  </si>
-  <si>
-    <t>TaskID</t>
-  </si>
-  <si>
-    <t>任务杀怪表</t>
-  </si>
-  <si>
     <t>BuildingID</t>
   </si>
   <si>
     <t>BuildingGUID</t>
   </si>
   <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>PosX</t>
+  </si>
+  <si>
+    <t>PosY</t>
+  </si>
+  <si>
+    <t>PosZ</t>
+  </si>
+  <si>
+    <t>StateStartTime</t>
+  </si>
+  <si>
+    <t>StateEndTime</t>
+  </si>
+  <si>
+    <t>BuildingList</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>ItemID</t>
+  </si>
+  <si>
+    <t>LeftCount</t>
+  </si>
+  <si>
+    <t>OnceTime</t>
+  </si>
+  <si>
+    <t>OnceStartTime</t>
+  </si>
+  <si>
+    <t>BuildingProduce</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -254,114 +208,41 @@
   </si>
   <si>
     <t>Enable</t>
-  </si>
-  <si>
-    <t>BuildingList</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>State</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PosX</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PosY</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PosZ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BuildingGUID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>object</t>
-  </si>
-  <si>
-    <t>ItemID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LeftCount</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnceTime</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OnceStartTime</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>StateStartTime</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>StateEndTime</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BuildingProduce</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LoadPropertyFinish</t>
-  </si>
-  <si>
-    <t>TaskMonsterList</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color indexed="17"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color indexed="60"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="4">
@@ -373,12 +254,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor indexed="42"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -391,14 +274,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -406,34 +304,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="8">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="1" builtinId="26"/>
-    <cellStyle name="适中" xfId="2" builtinId="28"/>
+    <cellStyle name="好" xfId="1"/>
+    <cellStyle name="千位分隔" xfId="2" builtinId="3"/>
+    <cellStyle name="适中" xfId="3"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="百分比" xfId="6" builtinId="5"/>
+    <cellStyle name="货币[0]" xfId="7" builtinId="7"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -732,7 +625,6 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -765,14 +657,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="17.125" customWidth="1"/>
     <col min="2" max="3" width="7.375" customWidth="1"/>
@@ -784,7 +677,7 @@
     <col min="10" max="10" width="70.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -816,11 +709,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="b">
@@ -841,18 +734,18 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:10">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="b">
@@ -873,18 +766,18 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="b">
@@ -905,18 +798,18 @@
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:10">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="b">
@@ -937,18 +830,18 @@
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:10">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="b">
@@ -969,18 +862,18 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:10">
+      <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="b">
@@ -1001,18 +894,18 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:10">
+      <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="b">
@@ -1033,14 +926,14 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1065,14 +958,14 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1097,14 +990,14 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1129,14 +1022,14 @@
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1161,18 +1054,18 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C13" t="b">
@@ -1193,171 +1086,33 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F12 F14:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="16.125" customWidth="1"/>
-    <col min="2" max="3" width="7.125" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="8" max="8" width="9.375" customWidth="1"/>
-    <col min="9" max="9" width="17.75" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="12.75" customWidth="1"/>
-    <col min="13" max="14" width="22.75" customWidth="1"/>
-    <col min="15" max="15" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L1:O1048576">
-      <formula1>"int,float,string,object"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="16.125" customWidth="1"/>
     <col min="2" max="3" width="7.125" customWidth="1"/>
@@ -1368,330 +1123,331 @@
     <col min="10" max="10" width="19" customWidth="1"/>
     <col min="12" max="12" width="12.75" customWidth="1"/>
     <col min="13" max="13" width="13.875" customWidth="1"/>
-    <col min="15" max="15" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.625" customWidth="1"/>
+    <col min="16" max="16" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+      <c r="R1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="1">
+        <v>128</v>
+      </c>
+      <c r="C2" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="2">
-        <v>128</v>
-      </c>
-      <c r="C2" s="2">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>52</v>
+      <c r="N2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1:M1 L42:L1048576 O1:Q1"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M2 L2:L41 O2:Q2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M2 O2:Q2 L2:L41">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D1:F1048576">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1:M1 O1:Q1 L42:L1048576"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
       <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:C1048576">
-      <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+      <formula1>0</formula1>
+    </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="16.125" customWidth="1"/>
     <col min="2" max="2" width="7.125" customWidth="1"/>
-    <col min="3" max="3" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5" customWidth="1"/>
+    <col min="4" max="4" width="7.5" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="7" width="5.5" customWidth="1"/>
+    <col min="8" max="8" width="6.5" customWidth="1"/>
+    <col min="9" max="9" width="13.875" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="5.5" customWidth="1"/>
+    <col min="12" max="12" width="13.875" customWidth="1"/>
+    <col min="13" max="13" width="7.5" customWidth="1"/>
+    <col min="14" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="9.5" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:16">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="L1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1">
         <v>128</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="D2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="4" t="s">
+      <c r="N2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L2 N2:P2">
+      <formula1>"int,float,string,object"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="L1 N1:P1"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2">
       <formula1>"int,float,string,object"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C2 B1:B1048576">
-      <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2 D1:F2">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N2:P2 L2">
-      <formula1>"int,float,string,object"</formula1>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576 C1:C2">
+      <formula1>0</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="N1:P1 L1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1"/>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="8.25" customWidth="1"/>
     <col min="2" max="2" width="12.75" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>